<commit_message>
edit report template & document origin
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
@@ -20,15 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">Tax Exemption Report</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">Tax Exemption</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
   </si>
   <si>
     <t xml:space="preserve">Taxbranch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Invoice</t>
@@ -77,11 +83,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +116,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -138,19 +153,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -194,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,35 +235,39 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,10 +348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -378,7 +390,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" s="7" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -390,12 +402,11 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -407,90 +418,126 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-    </row>
-    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="E8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AMJ6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="J8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="AMJ7" s="5"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update Tax exemption receipt Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
-    <t xml:space="preserve">Tax Exemption</t>
+    <t xml:space="preserve">Tax Exemption Report</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
@@ -85,7 +85,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
   </numFmts>
@@ -202,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +231,14 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,7 +255,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,180 +363,186 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="14" style="5" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="17.4"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" s="7" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" s="9" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="0"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="0"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="0"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="0"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
[IMP] Adjust Tax exemption report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_tax_exemption_receipt.xlsx
@@ -83,11 +83,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -202,12 +203,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,8 +216,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -231,11 +236,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,7 +248,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,27 +260,27 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,186 +368,187 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="3" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="14" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="14" style="6" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="17.4"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" s="9" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+    <row r="1" s="10" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" s="10" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="8"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="8"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="8"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>